<commit_message>
Rename spec files to take out blanks, for sanity
</commit_message>
<xml_diff>
--- a/doc/hualian-sensors.xlsx
+++ b/doc/hualian-sensors.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12788" windowHeight="9563" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12788" windowHeight="9563"/>
   </bookViews>
   <sheets>
     <sheet name="Site Map" sheetId="9" r:id="rId1"/>
@@ -3829,7 +3829,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -4076,35 +4076,35 @@
         <v>42651</v>
       </c>
       <c r="F2" s="15" t="str">
-        <f>IF(AND(F$1&lt;=$C2, $C2&lt;F$1+7), "X","")</f>
+        <f t="shared" ref="F2:M11" si="0">IF(AND(F$1&lt;=$C2, $C2&lt;F$1+7), "X","")</f>
         <v>X</v>
       </c>
       <c r="G2" s="15" t="str">
-        <f>IF(AND(G$1&lt;=$C2, $C2&lt;G$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H2" s="15" t="str">
-        <f>IF(AND(H$1&lt;=$C2, $C2&lt;H$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I2" s="15" t="str">
-        <f>IF(AND(I$1&lt;=$C2, $C2&lt;I$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J2" s="15" t="str">
-        <f>IF(AND(J$1&lt;=$C2, $C2&lt;J$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K2" s="15" t="str">
-        <f>IF(AND(K$1&lt;=$C2, $C2&lt;K$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="L2" s="15" t="str">
-        <f>IF(AND(L$1&lt;=$C2, $C2&lt;L$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M2" s="15" t="str">
-        <f>IF(AND(M$1&lt;=$C2, $C2&lt;M$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -4119,35 +4119,35 @@
         <v>87</v>
       </c>
       <c r="F3" s="15" t="str">
-        <f>IF(AND(F$1&lt;=$C3, $C3&lt;F$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v>X</v>
       </c>
       <c r="G3" s="15" t="str">
-        <f>IF(AND(G$1&lt;=$C3, $C3&lt;G$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H3" s="15" t="str">
-        <f>IF(AND(H$1&lt;=$C3, $C3&lt;H$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I3" s="15" t="str">
-        <f>IF(AND(I$1&lt;=$C3, $C3&lt;I$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J3" s="15" t="str">
-        <f>IF(AND(J$1&lt;=$C3, $C3&lt;J$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K3" s="15" t="str">
-        <f>IF(AND(K$1&lt;=$C3, $C3&lt;K$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="L3" s="15" t="str">
-        <f>IF(AND(L$1&lt;=$C3, $C3&lt;L$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M3" s="15" t="str">
-        <f>IF(AND(M$1&lt;=$C3, $C3&lt;M$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -4162,35 +4162,35 @@
         <v>83</v>
       </c>
       <c r="F4" s="15" t="str">
-        <f>IF(AND(F$1&lt;=$C4, $C4&lt;F$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v>X</v>
       </c>
       <c r="G4" s="15" t="str">
-        <f>IF(AND(G$1&lt;=$C4, $C4&lt;G$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H4" s="15" t="str">
-        <f>IF(AND(H$1&lt;=$C4, $C4&lt;H$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I4" s="15" t="str">
-        <f>IF(AND(I$1&lt;=$C4, $C4&lt;I$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J4" s="15" t="str">
-        <f>IF(AND(J$1&lt;=$C4, $C4&lt;J$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K4" s="15" t="str">
-        <f>IF(AND(K$1&lt;=$C4, $C4&lt;K$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="L4" s="15" t="str">
-        <f>IF(AND(L$1&lt;=$C4, $C4&lt;L$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M4" s="15" t="str">
-        <f>IF(AND(M$1&lt;=$C4, $C4&lt;M$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -4205,35 +4205,35 @@
         <v>87</v>
       </c>
       <c r="F5" s="15" t="str">
-        <f>IF(AND(F$1&lt;=$C5, $C5&lt;F$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v>X</v>
       </c>
       <c r="G5" s="15" t="str">
-        <f>IF(AND(G$1&lt;=$C5, $C5&lt;G$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H5" s="15" t="str">
-        <f>IF(AND(H$1&lt;=$C5, $C5&lt;H$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I5" s="15" t="str">
-        <f>IF(AND(I$1&lt;=$C5, $C5&lt;I$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J5" s="15" t="str">
-        <f>IF(AND(J$1&lt;=$C5, $C5&lt;J$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K5" s="15" t="str">
-        <f>IF(AND(K$1&lt;=$C5, $C5&lt;K$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="L5" s="15" t="str">
-        <f>IF(AND(L$1&lt;=$C5, $C5&lt;L$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M5" s="15" t="str">
-        <f>IF(AND(M$1&lt;=$C5, $C5&lt;M$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -4248,35 +4248,35 @@
         <v>94</v>
       </c>
       <c r="F6" s="15" t="str">
-        <f>IF(AND(F$1&lt;=$C6, $C6&lt;F$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v>X</v>
       </c>
       <c r="G6" s="15" t="str">
-        <f>IF(AND(G$1&lt;=$C6, $C6&lt;G$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H6" s="15" t="str">
-        <f>IF(AND(H$1&lt;=$C6, $C6&lt;H$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I6" s="15" t="str">
-        <f>IF(AND(I$1&lt;=$C6, $C6&lt;I$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J6" s="15" t="str">
-        <f>IF(AND(J$1&lt;=$C6, $C6&lt;J$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K6" s="15" t="str">
-        <f>IF(AND(K$1&lt;=$C6, $C6&lt;K$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="L6" s="15" t="str">
-        <f>IF(AND(L$1&lt;=$C6, $C6&lt;L$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M6" s="15" t="str">
-        <f>IF(AND(M$1&lt;=$C6, $C6&lt;M$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -4291,35 +4291,35 @@
         <v>83</v>
       </c>
       <c r="F7" s="15" t="str">
-        <f>IF(AND(F$1&lt;=$C7, $C7&lt;F$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G7" s="15" t="str">
-        <f>IF(AND(G$1&lt;=$C7, $C7&lt;G$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v>X</v>
       </c>
       <c r="H7" s="15" t="str">
-        <f>IF(AND(H$1&lt;=$C7, $C7&lt;H$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I7" s="15" t="str">
-        <f>IF(AND(I$1&lt;=$C7, $C7&lt;I$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J7" s="15" t="str">
-        <f>IF(AND(J$1&lt;=$C7, $C7&lt;J$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K7" s="15" t="str">
-        <f>IF(AND(K$1&lt;=$C7, $C7&lt;K$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="L7" s="15" t="str">
-        <f>IF(AND(L$1&lt;=$C7, $C7&lt;L$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M7" s="15" t="str">
-        <f>IF(AND(M$1&lt;=$C7, $C7&lt;M$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -4334,35 +4334,35 @@
         <v>83</v>
       </c>
       <c r="F8" s="15" t="str">
-        <f>IF(AND(F$1&lt;=$C8, $C8&lt;F$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G8" s="15" t="str">
-        <f>IF(AND(G$1&lt;=$C8, $C8&lt;G$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v>X</v>
       </c>
       <c r="H8" s="15" t="str">
-        <f>IF(AND(H$1&lt;=$C8, $C8&lt;H$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I8" s="15" t="str">
-        <f>IF(AND(I$1&lt;=$C8, $C8&lt;I$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J8" s="15" t="str">
-        <f>IF(AND(J$1&lt;=$C8, $C8&lt;J$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K8" s="15" t="str">
-        <f>IF(AND(K$1&lt;=$C8, $C8&lt;K$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="L8" s="15" t="str">
-        <f>IF(AND(L$1&lt;=$C8, $C8&lt;L$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M8" s="15" t="str">
-        <f>IF(AND(M$1&lt;=$C8, $C8&lt;M$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -4377,35 +4377,35 @@
         <v>83</v>
       </c>
       <c r="F9" s="15" t="str">
-        <f>IF(AND(F$1&lt;=$C9, $C9&lt;F$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G9" s="15" t="str">
-        <f>IF(AND(G$1&lt;=$C9, $C9&lt;G$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v>X</v>
       </c>
       <c r="H9" s="15" t="str">
-        <f>IF(AND(H$1&lt;=$C9, $C9&lt;H$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I9" s="15" t="str">
-        <f>IF(AND(I$1&lt;=$C9, $C9&lt;I$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J9" s="15" t="str">
-        <f>IF(AND(J$1&lt;=$C9, $C9&lt;J$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K9" s="15" t="str">
-        <f>IF(AND(K$1&lt;=$C9, $C9&lt;K$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="L9" s="15" t="str">
-        <f>IF(AND(L$1&lt;=$C9, $C9&lt;L$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M9" s="15" t="str">
-        <f>IF(AND(M$1&lt;=$C9, $C9&lt;M$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -4420,35 +4420,35 @@
         <v>83</v>
       </c>
       <c r="F10" s="15" t="str">
-        <f>IF(AND(F$1&lt;=$C10, $C10&lt;F$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G10" s="15" t="str">
-        <f>IF(AND(G$1&lt;=$C10, $C10&lt;G$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v>X</v>
       </c>
       <c r="H10" s="15" t="str">
-        <f>IF(AND(H$1&lt;=$C10, $C10&lt;H$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I10" s="15" t="str">
-        <f>IF(AND(I$1&lt;=$C10, $C10&lt;I$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J10" s="15" t="str">
-        <f>IF(AND(J$1&lt;=$C10, $C10&lt;J$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K10" s="15" t="str">
-        <f>IF(AND(K$1&lt;=$C10, $C10&lt;K$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="L10" s="15" t="str">
-        <f>IF(AND(L$1&lt;=$C10, $C10&lt;L$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M10" s="15" t="str">
-        <f>IF(AND(M$1&lt;=$C10, $C10&lt;M$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -4464,35 +4464,35 @@
       </c>
       <c r="E11" s="17"/>
       <c r="F11" s="15" t="str">
-        <f>IF(AND(F$1&lt;=$C11, $C11&lt;F$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="G11" s="15" t="str">
-        <f>IF(AND(G$1&lt;=$C11, $C11&lt;G$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v>X</v>
       </c>
       <c r="H11" s="15" t="str">
-        <f>IF(AND(H$1&lt;=$C11, $C11&lt;H$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I11" s="15" t="str">
-        <f>IF(AND(I$1&lt;=$C11, $C11&lt;I$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J11" s="15" t="str">
-        <f>IF(AND(J$1&lt;=$C11, $C11&lt;J$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K11" s="15" t="str">
-        <f>IF(AND(K$1&lt;=$C11, $C11&lt;K$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="L11" s="15" t="str">
-        <f>IF(AND(L$1&lt;=$C11, $C11&lt;L$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M11" s="15" t="str">
-        <f>IF(AND(M$1&lt;=$C11, $C11&lt;M$1+7), "X","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -4507,35 +4507,35 @@
         <v>94</v>
       </c>
       <c r="F12" s="15" t="str">
-        <f>IF(AND(F$1&lt;=$C12, $C12&lt;F$1+7), "X","")</f>
+        <f t="shared" ref="F12:M26" si="1">IF(AND(F$1&lt;=$C12, $C12&lt;F$1+7), "X","")</f>
         <v/>
       </c>
       <c r="G12" s="15" t="str">
-        <f>IF(AND(G$1&lt;=$C12, $C12&lt;G$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H12" s="15" t="str">
-        <f>IF(AND(H$1&lt;=$C12, $C12&lt;H$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="I12" s="15" t="str">
-        <f>IF(AND(I$1&lt;=$C12, $C12&lt;I$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J12" s="15" t="str">
-        <f>IF(AND(J$1&lt;=$C12, $C12&lt;J$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K12" s="15" t="str">
-        <f>IF(AND(K$1&lt;=$C12, $C12&lt;K$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="L12" s="15" t="str">
-        <f>IF(AND(L$1&lt;=$C12, $C12&lt;L$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M12" s="15" t="str">
-        <f>IF(AND(M$1&lt;=$C12, $C12&lt;M$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -4550,35 +4550,35 @@
         <v>87</v>
       </c>
       <c r="F13" s="15" t="str">
-        <f>IF(AND(F$1&lt;=$C13, $C13&lt;F$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G13" s="15" t="str">
-        <f>IF(AND(G$1&lt;=$C13, $C13&lt;G$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H13" s="15" t="str">
-        <f>IF(AND(H$1&lt;=$C13, $C13&lt;H$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="I13" s="15" t="str">
-        <f>IF(AND(I$1&lt;=$C13, $C13&lt;I$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J13" s="15" t="str">
-        <f>IF(AND(J$1&lt;=$C13, $C13&lt;J$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K13" s="15" t="str">
-        <f>IF(AND(K$1&lt;=$C13, $C13&lt;K$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="L13" s="15" t="str">
-        <f>IF(AND(L$1&lt;=$C13, $C13&lt;L$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M13" s="15" t="str">
-        <f>IF(AND(M$1&lt;=$C13, $C13&lt;M$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -4593,35 +4593,35 @@
         <v>83</v>
       </c>
       <c r="F14" s="15" t="str">
-        <f>IF(AND(F$1&lt;=$C14, $C14&lt;F$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G14" s="15" t="str">
-        <f>IF(AND(G$1&lt;=$C14, $C14&lt;G$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H14" s="15" t="str">
-        <f>IF(AND(H$1&lt;=$C14, $C14&lt;H$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I14" s="15" t="str">
-        <f>IF(AND(I$1&lt;=$C14, $C14&lt;I$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="J14" s="15" t="str">
-        <f>IF(AND(J$1&lt;=$C14, $C14&lt;J$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K14" s="15" t="str">
-        <f>IF(AND(K$1&lt;=$C14, $C14&lt;K$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="L14" s="15" t="str">
-        <f>IF(AND(L$1&lt;=$C14, $C14&lt;L$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M14" s="15" t="str">
-        <f>IF(AND(M$1&lt;=$C14, $C14&lt;M$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -4636,35 +4636,35 @@
         <v>83</v>
       </c>
       <c r="F15" s="15" t="str">
-        <f>IF(AND(F$1&lt;=$C15, $C15&lt;F$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G15" s="15" t="str">
-        <f>IF(AND(G$1&lt;=$C15, $C15&lt;G$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H15" s="15" t="str">
-        <f>IF(AND(H$1&lt;=$C15, $C15&lt;H$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I15" s="15" t="str">
-        <f>IF(AND(I$1&lt;=$C15, $C15&lt;I$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="J15" s="15" t="str">
-        <f>IF(AND(J$1&lt;=$C15, $C15&lt;J$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K15" s="15" t="str">
-        <f>IF(AND(K$1&lt;=$C15, $C15&lt;K$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="L15" s="15" t="str">
-        <f>IF(AND(L$1&lt;=$C15, $C15&lt;L$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M15" s="15" t="str">
-        <f>IF(AND(M$1&lt;=$C15, $C15&lt;M$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -4679,35 +4679,35 @@
         <v>83</v>
       </c>
       <c r="F16" s="15" t="str">
-        <f>IF(AND(F$1&lt;=$C16, $C16&lt;F$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G16" s="15" t="str">
-        <f>IF(AND(G$1&lt;=$C16, $C16&lt;G$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H16" s="15" t="str">
-        <f>IF(AND(H$1&lt;=$C16, $C16&lt;H$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I16" s="15" t="str">
-        <f>IF(AND(I$1&lt;=$C16, $C16&lt;I$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="J16" s="15" t="str">
-        <f>IF(AND(J$1&lt;=$C16, $C16&lt;J$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K16" s="15" t="str">
-        <f>IF(AND(K$1&lt;=$C16, $C16&lt;K$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="L16" s="15" t="str">
-        <f>IF(AND(L$1&lt;=$C16, $C16&lt;L$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M16" s="15" t="str">
-        <f>IF(AND(M$1&lt;=$C16, $C16&lt;M$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -4725,35 +4725,35 @@
         <v>96</v>
       </c>
       <c r="F17" s="15" t="str">
-        <f>IF(AND(F$1&lt;=$C17, $C17&lt;F$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G17" s="15" t="str">
-        <f>IF(AND(G$1&lt;=$C17, $C17&lt;G$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H17" s="15" t="str">
-        <f>IF(AND(H$1&lt;=$C17, $C17&lt;H$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I17" s="15" t="str">
-        <f>IF(AND(I$1&lt;=$C17, $C17&lt;I$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J17" s="15" t="str">
-        <f>IF(AND(J$1&lt;=$C17, $C17&lt;J$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="K17" s="15" t="str">
-        <f>IF(AND(K$1&lt;=$C17, $C17&lt;K$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="L17" s="15" t="str">
-        <f>IF(AND(L$1&lt;=$C17, $C17&lt;L$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M17" s="15" t="str">
-        <f>IF(AND(M$1&lt;=$C17, $C17&lt;M$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -4768,35 +4768,35 @@
         <v>83</v>
       </c>
       <c r="F18" s="15" t="str">
-        <f>IF(AND(F$1&lt;=$C18, $C18&lt;F$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G18" s="15" t="str">
-        <f>IF(AND(G$1&lt;=$C18, $C18&lt;G$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H18" s="15" t="str">
-        <f>IF(AND(H$1&lt;=$C18, $C18&lt;H$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I18" s="15" t="str">
-        <f>IF(AND(I$1&lt;=$C18, $C18&lt;I$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J18" s="15" t="str">
-        <f>IF(AND(J$1&lt;=$C18, $C18&lt;J$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="K18" s="15" t="str">
-        <f>IF(AND(K$1&lt;=$C18, $C18&lt;K$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="L18" s="15" t="str">
-        <f>IF(AND(L$1&lt;=$C18, $C18&lt;L$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M18" s="15" t="str">
-        <f>IF(AND(M$1&lt;=$C18, $C18&lt;M$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -4812,35 +4812,35 @@
         <v>99</v>
       </c>
       <c r="F19" s="15" t="str">
-        <f>IF(AND(F$1&lt;=$C19, $C19&lt;F$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G19" s="15" t="str">
-        <f>IF(AND(G$1&lt;=$C19, $C19&lt;G$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H19" s="15" t="str">
-        <f>IF(AND(H$1&lt;=$C19, $C19&lt;H$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I19" s="15" t="str">
-        <f>IF(AND(I$1&lt;=$C19, $C19&lt;I$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J19" s="15" t="str">
-        <f>IF(AND(J$1&lt;=$C19, $C19&lt;J$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="K19" s="15" t="str">
-        <f>IF(AND(K$1&lt;=$C19, $C19&lt;K$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="L19" s="15" t="str">
-        <f>IF(AND(L$1&lt;=$C19, $C19&lt;L$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M19" s="15" t="str">
-        <f>IF(AND(M$1&lt;=$C19, $C19&lt;M$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -4855,35 +4855,35 @@
         <v>87</v>
       </c>
       <c r="F20" s="15" t="str">
-        <f>IF(AND(F$1&lt;=$C20, $C20&lt;F$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G20" s="15" t="str">
-        <f>IF(AND(G$1&lt;=$C20, $C20&lt;G$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H20" s="15" t="str">
-        <f>IF(AND(H$1&lt;=$C20, $C20&lt;H$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I20" s="15" t="str">
-        <f>IF(AND(I$1&lt;=$C20, $C20&lt;I$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J20" s="15" t="str">
-        <f>IF(AND(J$1&lt;=$C20, $C20&lt;J$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K20" s="15" t="str">
-        <f>IF(AND(K$1&lt;=$C20, $C20&lt;K$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="L20" s="15" t="str">
-        <f>IF(AND(L$1&lt;=$C20, $C20&lt;L$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M20" s="15" t="str">
-        <f>IF(AND(M$1&lt;=$C20, $C20&lt;M$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -4899,35 +4899,35 @@
         <v>87</v>
       </c>
       <c r="F21" s="15" t="str">
-        <f>IF(AND(F$1&lt;=$C21, $C21&lt;F$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G21" s="15" t="str">
-        <f>IF(AND(G$1&lt;=$C21, $C21&lt;G$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H21" s="15" t="str">
-        <f>IF(AND(H$1&lt;=$C21, $C21&lt;H$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I21" s="15" t="str">
-        <f>IF(AND(I$1&lt;=$C21, $C21&lt;I$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J21" s="15" t="str">
-        <f>IF(AND(J$1&lt;=$C21, $C21&lt;J$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K21" s="15" t="str">
-        <f>IF(AND(K$1&lt;=$C21, $C21&lt;K$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="L21" s="15" t="str">
-        <f>IF(AND(L$1&lt;=$C21, $C21&lt;L$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="M21" s="15" t="str">
-        <f>IF(AND(M$1&lt;=$C21, $C21&lt;M$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -4942,35 +4942,35 @@
         <v>87</v>
       </c>
       <c r="F22" s="15" t="str">
-        <f>IF(AND(F$1&lt;=$C22, $C22&lt;F$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G22" s="15" t="str">
-        <f>IF(AND(G$1&lt;=$C22, $C22&lt;G$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H22" s="15" t="str">
-        <f>IF(AND(H$1&lt;=$C22, $C22&lt;H$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I22" s="15" t="str">
-        <f>IF(AND(I$1&lt;=$C22, $C22&lt;I$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J22" s="15" t="str">
-        <f>IF(AND(J$1&lt;=$C22, $C22&lt;J$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K22" s="15" t="str">
-        <f>IF(AND(K$1&lt;=$C22, $C22&lt;K$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="L22" s="15" t="str">
-        <f>IF(AND(L$1&lt;=$C22, $C22&lt;L$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="M22" s="15" t="str">
-        <f>IF(AND(M$1&lt;=$C22, $C22&lt;M$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -4985,137 +4985,137 @@
         <v>87</v>
       </c>
       <c r="F23" s="15" t="str">
-        <f>IF(AND(F$1&lt;=$C23, $C23&lt;F$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G23" s="15" t="str">
-        <f>IF(AND(G$1&lt;=$C23, $C23&lt;G$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H23" s="15" t="str">
-        <f>IF(AND(H$1&lt;=$C23, $C23&lt;H$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I23" s="15" t="str">
-        <f>IF(AND(I$1&lt;=$C23, $C23&lt;I$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J23" s="15" t="str">
-        <f>IF(AND(J$1&lt;=$C23, $C23&lt;J$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K23" s="15" t="str">
-        <f>IF(AND(K$1&lt;=$C23, $C23&lt;K$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="L23" s="15" t="str">
-        <f>IF(AND(L$1&lt;=$C23, $C23&lt;L$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="M23" s="15" t="str">
-        <f>IF(AND(M$1&lt;=$C23, $C23&lt;M$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.45">
       <c r="F24" s="15" t="str">
-        <f>IF(AND(F$1&lt;=$C24, $C24&lt;F$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G24" s="15" t="str">
-        <f>IF(AND(G$1&lt;=$C24, $C24&lt;G$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H24" s="15" t="str">
-        <f>IF(AND(H$1&lt;=$C24, $C24&lt;H$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I24" s="15" t="str">
-        <f>IF(AND(I$1&lt;=$C24, $C24&lt;I$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J24" s="15" t="str">
-        <f>IF(AND(J$1&lt;=$C24, $C24&lt;J$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K24" s="15" t="str">
-        <f>IF(AND(K$1&lt;=$C24, $C24&lt;K$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="L24" s="15" t="str">
-        <f>IF(AND(L$1&lt;=$C24, $C24&lt;L$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M24" s="15" t="str">
-        <f>IF(AND(M$1&lt;=$C24, $C24&lt;M$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.45">
       <c r="F25" s="15" t="str">
-        <f>IF(AND(F$1&lt;=$C25, $C25&lt;F$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G25" s="15" t="str">
-        <f>IF(AND(G$1&lt;=$C25, $C25&lt;G$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H25" s="15" t="str">
-        <f>IF(AND(H$1&lt;=$C25, $C25&lt;H$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I25" s="15" t="str">
-        <f>IF(AND(I$1&lt;=$C25, $C25&lt;I$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J25" s="15" t="str">
-        <f>IF(AND(J$1&lt;=$C25, $C25&lt;J$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K25" s="15" t="str">
-        <f>IF(AND(K$1&lt;=$C25, $C25&lt;K$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="L25" s="15" t="str">
-        <f>IF(AND(L$1&lt;=$C25, $C25&lt;L$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M25" s="15" t="str">
-        <f>IF(AND(M$1&lt;=$C25, $C25&lt;M$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.45">
       <c r="F26" s="15" t="str">
-        <f>IF(AND(F$1&lt;=$C26, $C26&lt;F$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G26" s="15" t="str">
-        <f>IF(AND(G$1&lt;=$C26, $C26&lt;G$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H26" s="15" t="str">
-        <f>IF(AND(H$1&lt;=$C26, $C26&lt;H$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I26" s="15" t="str">
-        <f>IF(AND(I$1&lt;=$C26, $C26&lt;I$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J26" s="15" t="str">
-        <f>IF(AND(J$1&lt;=$C26, $C26&lt;J$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K26" s="15" t="str">
-        <f>IF(AND(K$1&lt;=$C26, $C26&lt;K$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="L26" s="15" t="str">
-        <f>IF(AND(L$1&lt;=$C26, $C26&lt;L$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M26" s="15" t="str">
-        <f>IF(AND(M$1&lt;=$C26, $C26&lt;M$1+7), "X","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -5138,7 +5138,7 @@
   <dimension ref="B1:J12"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6179,8 +6179,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:W38"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Capture changes to spreadsheet and mindmap
</commit_message>
<xml_diff>
--- a/doc/hualian-sensors.xlsx
+++ b/doc/hualian-sensors.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mcci\Marketing\TheThingsNetwork\projects\hualian\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mcci\client\anatolian\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12788" windowHeight="9563" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12790" windowHeight="7750" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Site Map" sheetId="9" r:id="rId1"/>
@@ -22,9 +22,10 @@
     <sheet name="Network Diagram" sheetId="8" r:id="rId8"/>
     <sheet name="Pond Sensor" sheetId="2" r:id="rId9"/>
     <sheet name="Schedule" sheetId="12" r:id="rId10"/>
+    <sheet name="Minutes 10-27" sheetId="13" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Schedule!$B$1:$M$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Schedule!$B$1:$M$28</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="110">
   <si>
     <t>Basic Feather M0 Sensor</t>
   </si>
@@ -339,6 +340,36 @@
   </si>
   <si>
     <t>Fedex</t>
+  </si>
+  <si>
+    <t>Meeting 10/27</t>
+  </si>
+  <si>
+    <t>Ammonia sensors will not be integrated into the first phase</t>
+  </si>
+  <si>
+    <t>Seaweed room: we'll include temperature, humidity, and seaweed tank water temperature</t>
+  </si>
+  <si>
+    <t>Mushroom, gh -- all done</t>
+  </si>
+  <si>
+    <t>We'll send a base image of VM to Hualian for them to do a test install - post on dropbox, and they can download</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+  <si>
+    <t>Amy to provide shipping method</t>
+  </si>
+  <si>
+    <t>MCCI to ship mid-week</t>
+  </si>
+  <si>
+    <t>Test server posted &amp; email to Amy</t>
+  </si>
+  <si>
+    <t>DC connector spec for Conduit for Amy (photo and spec if possible)</t>
   </si>
 </sst>
 </file>
@@ -436,7 +467,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -479,6 +510,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -2080,8 +2120,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1060450" y="2616200"/>
-          <a:ext cx="2368550" cy="3289300"/>
+          <a:off x="1047750" y="2660650"/>
+          <a:ext cx="2317750" cy="3346450"/>
           <a:chOff x="1041400" y="2178050"/>
           <a:chExt cx="2292350" cy="3346450"/>
         </a:xfrm>
@@ -3832,7 +3872,7 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="49" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -3847,22 +3887,22 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M26"/>
+  <dimension ref="B1:M28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="19.46484375" style="11" customWidth="1"/>
-    <col min="3" max="3" width="10.86328125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="9.06640625" style="15"/>
-    <col min="5" max="5" width="20.265625" customWidth="1"/>
-    <col min="6" max="13" width="9.9296875" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.453125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="9.08984375" style="15"/>
+    <col min="5" max="5" width="20.26953125" customWidth="1"/>
+    <col min="6" max="13" width="9.90625" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B1" s="10" t="s">
         <v>72</v>
       </c>
@@ -3900,7 +3940,7 @@
         <v>42695</v>
       </c>
     </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B2" s="11" t="s">
         <v>73</v>
       </c>
@@ -3940,7 +3980,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
         <v>90</v>
       </c>
@@ -3983,7 +4023,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B4" s="11" t="s">
         <v>81</v>
       </c>
@@ -4026,7 +4066,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B5" s="11" t="s">
         <v>92</v>
       </c>
@@ -4069,7 +4109,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B6" s="11" t="s">
         <v>95</v>
       </c>
@@ -4112,7 +4152,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B7" s="11" t="s">
         <v>88</v>
       </c>
@@ -4155,7 +4195,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B8" s="11" t="s">
         <v>74</v>
       </c>
@@ -4198,7 +4238,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B9" s="11" t="s">
         <v>75</v>
       </c>
@@ -4241,7 +4281,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="2:13" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B10" s="11" t="s">
         <v>98</v>
       </c>
@@ -4284,7 +4324,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B11" s="11" t="s">
         <v>86</v>
       </c>
@@ -4328,7 +4368,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="2:13" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B12" s="11" t="s">
         <v>93</v>
       </c>
@@ -4339,7 +4379,7 @@
         <v>94</v>
       </c>
       <c r="F12" s="15" t="str">
-        <f t="shared" ref="F12:M26" si="1">IF(AND(F$1&lt;=$C12, $C12&lt;F$1+7), "X","")</f>
+        <f t="shared" ref="F12:M28" si="1">IF(AND(F$1&lt;=$C12, $C12&lt;F$1+7), "X","")</f>
         <v/>
       </c>
       <c r="G12" s="15" t="str">
@@ -4371,7 +4411,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B13" s="11" t="s">
         <v>97</v>
       </c>
@@ -4414,12 +4454,12 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="2:13" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B14" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C14" s="13">
-        <v>42667</v>
+      <c r="C14" s="20">
+        <v>42674</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>83</v>
@@ -4438,12 +4478,12 @@
       </c>
       <c r="I14" s="15" t="str">
         <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J14" s="15" t="str">
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
-      <c r="J14" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
       <c r="K14" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -4457,12 +4497,12 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="2:13" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:13" ht="58" x14ac:dyDescent="0.35">
       <c r="B15" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C15" s="13">
-        <v>42672</v>
+        <v>109</v>
+      </c>
+      <c r="C15" s="20">
+        <v>42674</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>83</v>
@@ -4481,12 +4521,12 @@
       </c>
       <c r="I15" s="15" t="str">
         <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J15" s="15" t="str">
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
-      <c r="J15" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
       <c r="K15" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -4500,62 +4540,59 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B16" s="11" t="s">
-        <v>77</v>
+        <v>108</v>
       </c>
       <c r="C16" s="13">
+        <v>42671</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="F16" s="15" t="str">
+        <f>IF(AND(F$1&lt;=$C16, $C16&lt;F$1+7), "X","")</f>
+        <v/>
+      </c>
+      <c r="G16" s="15" t="str">
+        <f>IF(AND(G$1&lt;=$C16, $C16&lt;G$1+7), "X","")</f>
+        <v/>
+      </c>
+      <c r="H16" s="15" t="str">
+        <f>IF(AND(H$1&lt;=$C16, $C16&lt;H$1+7), "X","")</f>
+        <v/>
+      </c>
+      <c r="I16" s="15" t="str">
+        <f>IF(AND(I$1&lt;=$C16, $C16&lt;I$1+7), "X","")</f>
+        <v>X</v>
+      </c>
+      <c r="J16" s="15" t="str">
+        <f>IF(AND(J$1&lt;=$C16, $C16&lt;J$1+7), "X","")</f>
+        <v/>
+      </c>
+      <c r="K16" s="15" t="str">
+        <f>IF(AND(K$1&lt;=$C16, $C16&lt;K$1+7), "X","")</f>
+        <v/>
+      </c>
+      <c r="L16" s="15" t="str">
+        <f>IF(AND(L$1&lt;=$C16, $C16&lt;L$1+7), "X","")</f>
+        <v/>
+      </c>
+      <c r="M16" s="15" t="str">
+        <f>IF(AND(M$1&lt;=$C16, $C16&lt;M$1+7), "X","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="2:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="B17" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="13">
         <v>42672</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="F16" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G16" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H16" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I16" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="J16" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K16" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="L16" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="M16" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="2:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B17" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C17" s="13">
-        <v>42674</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="E17" s="16" t="s">
-        <v>96</v>
-      </c>
       <c r="F17" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -4570,11 +4607,11 @@
       </c>
       <c r="I17" s="15" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J17" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>X</v>
+        <v/>
       </c>
       <c r="K17" s="15" t="str">
         <f t="shared" si="1"/>
@@ -4589,12 +4626,12 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:13" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B18" s="11" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C18" s="13">
-        <v>42674</v>
+        <v>42672</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>83</v>
@@ -4613,162 +4650,164 @@
       </c>
       <c r="I18" s="15" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J18" s="15" t="str">
         <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K18" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L18" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M18" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="2:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="B19" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="13">
+        <v>42674</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="F19" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G19" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H19" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I19" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J19" s="15" t="str">
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
-      <c r="K18" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="L18" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="M18" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B19" s="11" t="s">
+      <c r="K19" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L19" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M19" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B20" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="13">
+        <v>42674</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G20" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H20" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I20" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J20" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v>X</v>
+      </c>
+      <c r="K20" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L20" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M20" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B21" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="13">
-        <f>C18+3</f>
+      <c r="C21" s="13">
+        <f>C20+3</f>
         <v>42677</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D21" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="F19" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G19" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H19" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I19" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J19" s="15" t="str">
+      <c r="F21" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G21" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H21" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I21" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J21" s="15" t="str">
         <f t="shared" si="1"/>
         <v>X</v>
       </c>
-      <c r="K19" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="L19" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="M19" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="2:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B20" s="11" t="s">
+      <c r="K21" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L21" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M21" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="2:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="B22" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C22" s="13">
         <v>42684</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="F20" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G20" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H20" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I20" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J20" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K20" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="L20" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="M20" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B21" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="C21" s="13">
-        <f>C20+10</f>
-        <v>42694</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="F21" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G21" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H21" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I21" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J21" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K21" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="L21" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="M21" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B22" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="C22" s="13">
-        <v>42688</v>
       </c>
       <c r="D22" s="15" t="s">
         <v>87</v>
@@ -4795,23 +4834,24 @@
       </c>
       <c r="K22" s="15" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="L22" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>X</v>
+        <v/>
       </c>
       <c r="M22" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B23" s="11" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="C23" s="13">
-        <v>42692</v>
+        <f>C22+10</f>
+        <v>42694</v>
       </c>
       <c r="D23" s="15" t="s">
         <v>87</v>
@@ -4849,7 +4889,16 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B24" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="13">
+        <v>42688</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>87</v>
+      </c>
       <c r="F24" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -4876,14 +4925,23 @@
       </c>
       <c r="L24" s="15" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="M24" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B25" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="13">
+        <v>42692</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>87</v>
+      </c>
       <c r="F25" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -4910,14 +4968,14 @@
       </c>
       <c r="L25" s="15" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="M25" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.35">
       <c r="F26" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -4951,14 +5009,193 @@
         <v/>
       </c>
     </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="F27" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G27" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H27" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I27" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J27" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K27" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L27" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M27" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="F28" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G28" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H28" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I28" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J28" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K28" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L28" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M28" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:M26">
+  <autoFilter ref="B1:M28">
     <sortState ref="B2:M26">
       <sortCondition ref="C1:C26"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="8.7265625" style="18"/>
+    <col min="3" max="3" width="44.54296875" style="19" customWidth="1"/>
+    <col min="4" max="16384" width="8.7265625" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B2" s="18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D3" s="18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B4" s="15">
+        <v>1</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B5" s="15">
+        <v>2</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B6" s="15">
+        <v>3</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B7" s="15">
+        <v>4</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B8" s="15">
+        <v>5</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B9" s="15">
+        <v>6</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B10" s="15"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B11" s="15"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B12" s="15"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B13" s="15"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B14" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -4973,20 +5210,20 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="27.796875" customWidth="1"/>
-    <col min="3" max="3" width="12.19921875" customWidth="1"/>
-    <col min="7" max="7" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.81640625" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" customWidth="1"/>
+    <col min="7" max="7" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="2:10" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:10" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
         <v>43</v>
       </c>
@@ -5015,7 +5252,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>33</v>
       </c>
@@ -5050,7 +5287,7 @@
         <v>'Greenhouse Sensor'!$I$9</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>34</v>
       </c>
@@ -5085,7 +5322,7 @@
         <v>'Seaweed Sensor'!$I$7</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>35</v>
       </c>
@@ -5120,17 +5357,17 @@
         <v>'Mushroom Sensor'!$I$6</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>51</v>
       </c>
@@ -5148,7 +5385,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>56</v>
       </c>
@@ -5165,7 +5402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>54</v>
       </c>
@@ -5176,7 +5413,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>26</v>
       </c>
@@ -5208,17 +5445,17 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="79.33203125" customWidth="1"/>
+    <col min="2" max="2" width="79.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
         <v>46</v>
       </c>
@@ -5226,7 +5463,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>47</v>
       </c>
@@ -5261,17 +5498,17 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="33.19921875" customWidth="1"/>
+    <col min="3" max="3" width="33.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.35">
       <c r="J1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
@@ -5318,7 +5555,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="2:16" ht="14" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:16" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>1</v>
       </c>
@@ -5360,7 +5597,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>1</v>
       </c>
@@ -5405,7 +5642,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>1</v>
       </c>
@@ -5424,7 +5661,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>1</v>
       </c>
@@ -5443,7 +5680,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B7">
         <v>0</v>
       </c>
@@ -5479,7 +5716,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>1</v>
       </c>
@@ -5494,7 +5731,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>26</v>
       </c>
@@ -5529,17 +5766,17 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="8.796875" style="1"/>
-    <col min="3" max="3" width="33.19921875" customWidth="1"/>
-    <col min="5" max="5" width="8.796875" style="1"/>
-    <col min="6" max="6" width="12.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="35.46484375" customWidth="1"/>
-    <col min="8" max="8" width="12.796875" customWidth="1"/>
+    <col min="2" max="2" width="8.81640625" style="1"/>
+    <col min="3" max="3" width="33.1796875" customWidth="1"/>
+    <col min="5" max="5" width="8.81640625" style="1"/>
+    <col min="6" max="6" width="12.36328125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="35.453125" customWidth="1"/>
+    <col min="8" max="8" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
@@ -5586,7 +5823,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -5619,7 +5856,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B4" s="1">
         <v>1</v>
       </c>
@@ -5641,7 +5878,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -5669,7 +5906,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B6" s="1">
         <v>1</v>
       </c>
@@ -5687,7 +5924,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>26</v>
       </c>
@@ -5696,7 +5933,7 @@
         <v>109.95</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>58</v>
       </c>
@@ -5726,18 +5963,18 @@
   </sheetPr>
   <dimension ref="B2:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="8.796875" style="1"/>
-    <col min="3" max="3" width="14.59765625" customWidth="1"/>
-    <col min="10" max="16" width="8.796875" style="9"/>
+    <col min="2" max="2" width="8.81640625" style="1"/>
+    <col min="3" max="3" width="14.6328125" customWidth="1"/>
+    <col min="10" max="16" width="8.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:16" ht="29" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
@@ -5784,7 +6021,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="2:16" ht="14" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:16" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -5826,7 +6063,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B4" s="1">
         <v>1</v>
       </c>
@@ -5871,7 +6108,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -5907,7 +6144,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
@@ -5916,7 +6153,7 @@
         <v>149.94999999999999</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>60</v>
       </c>
@@ -5946,24 +6183,24 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>65</v>
       </c>
@@ -5971,17 +6208,17 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>69</v>
       </c>
@@ -5999,11 +6236,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" zoomScalePageLayoutView="200" workbookViewId="0">
+    <sheetView topLeftCell="F3" zoomScaleNormal="100" zoomScalePageLayoutView="200" workbookViewId="0">
       <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="77" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -6028,13 +6265,13 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="37.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="37.36328125" customWidth="1"/>
+    <col min="5" max="5" width="12.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
@@ -6081,7 +6318,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>1</v>
       </c>
@@ -6099,7 +6336,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>0</v>
       </c>
@@ -6120,7 +6357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>1</v>
       </c>
@@ -6144,7 +6381,7 @@
         <v>9.9499999999999993</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>1</v>
       </c>
@@ -6159,7 +6396,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>26</v>
       </c>

</xml_diff>